<commit_message>
Phase information matches, energy confirmed as non-matching.
</commit_message>
<xml_diff>
--- a/mpiData/Data.xlsx
+++ b/mpiData/Data.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="energies.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Stefan Air:Users:Stefan:Documents:School:UCSB 2014-2015:Winter Quarter:Cmpsc 140:Final Project:mpiData:MeltingTemp:energies.txt" delimited="0">
+    <textPr fileType="mac" sourceFile="Stefan Air:Users:Stefan:Documents:School:UCSB 2014-2015:Winter Quarter:Cmpsc 140:Final Project:mpiData:MeltingTemp:energies.txt" delimited="0">
       <textFields count="5">
         <textField/>
         <textField type="skip" position="4"/>
@@ -37,7 +37,7 @@
     </textPr>
   </connection>
   <connection id="2" name="pdInfo.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Stefan Air:Users:Stefan:Documents:School:UCSB 2014-2015:Winter Quarter:Cmpsc 140:Final Project:mpiData:PhaseDiagram:pdInfo.txt" delimited="0">
+    <textPr fileType="mac" sourceFile="Stefan Air:Users:Stefan:Documents:School:UCSB 2014-2015:Winter Quarter:Cmpsc 140:Final Project:mpiData:PhaseDiagram:pdInfo.txt" delimited="0">
       <textFields count="7">
         <textField/>
         <textField type="skip" position="4"/>
@@ -240,11 +240,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2081508856"/>
-        <c:axId val="2086560632"/>
+        <c:axId val="2076410728"/>
+        <c:axId val="2076413736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2081508856"/>
+        <c:axId val="2076410728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -254,12 +254,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086560632"/>
+        <c:crossAx val="2076413736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2086560632"/>
+        <c:axId val="2076413736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -270,7 +270,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081508856"/>
+        <c:crossAx val="2076410728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -313,7 +313,7 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -361,6 +361,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PhaseDiagram!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X1 (1-rich)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:dPt>
             <c:idx val="12"/>
             <c:bubble3D val="0"/>
@@ -372,10 +383,10 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>(PhaseDiagram!$B$2:$B$13,PhaseDiagram!$C$2:$C$13)</c:f>
+              <c:f>PhaseDiagram!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -411,52 +422,16 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.82</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.03</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(PhaseDiagram!$A$2:$A$13,PhaseDiagram!$A$2:$A$13)</c:f>
+              <c:f>PhaseDiagram!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.5</c:v>
                 </c:pt>
@@ -491,42 +466,6 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.05</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.55</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.95</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
                   <c:v>1.05</c:v>
                 </c:pt>
               </c:numCache>
@@ -535,8 +474,114 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PhaseDiagram!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>X1 (2-rich)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PhaseDiagram!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PhaseDiagram!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>PhaseDiagram!$A$18</c:f>
@@ -588,11 +633,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2116567320"/>
-        <c:axId val="2114693240"/>
+        <c:axId val="2077504216"/>
+        <c:axId val="2077513960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2116567320"/>
+        <c:axId val="2077504216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -604,12 +649,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114693240"/>
+        <c:crossAx val="2077513960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2114693240"/>
+        <c:axId val="2077513960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5"/>
@@ -621,16 +666,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116567320"/>
+        <c:crossAx val="2077504216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>

</xml_diff>